<commit_message>
tests reorganized in new directory
</commit_message>
<xml_diff>
--- a/testResults/plots.xlsx
+++ b/testResults/plots.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IncDelta" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="incD" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="IncD" localSheetId="3">incD!$A$2:$C$22</definedName>
+    <definedName name="IncD" localSheetId="3">incD!$A$2:$C$21</definedName>
     <definedName name="IncDelta" localSheetId="0">IncDelta!$A$2:$C$31</definedName>
     <definedName name="IncMlt" localSheetId="1">MLT!$A$2:$C$101</definedName>
     <definedName name="IncMrt" localSheetId="2">MRT!$A$2:$C$101</definedName>
@@ -30,7 +30,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="IncD.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="11" sourceFile="Macintosh HD:Users:daniel:Documents:Dokumente:EIT:Rennes:PEV:PEV_I:testResults:IncD.csv" decimal="," thousands="." tab="0" semicolon="1">
+    <textPr fileType="mac" firstRow="11" sourceFile="Macintosh HD:Users:daniel:Documents:Dokumente:EIT:Rennes:PEV:PEV_I:testResults:IncD.csv" decimal="," thousands="." tab="0" semicolon="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -39,7 +39,7 @@
     </textPr>
   </connection>
   <connection id="2" name="IncDelta.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="11" sourceFile="Macintosh HD:Users:daniel:Documents:Dokumente:EIT:Rennes:PEV:PEV_I:testResults:IncDelta.csv" decimal="," thousands="." tab="0" semicolon="1">
+    <textPr fileType="mac" firstRow="11" sourceFile="Macintosh HD:Users:daniel:Documents:Dokumente:EIT:Rennes:PEV:PEV_I:testResults:IncDelta.csv" decimal="," thousands="." tab="0" semicolon="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -48,7 +48,7 @@
     </textPr>
   </connection>
   <connection id="3" name="IncMlt.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="11" sourceFile="Macintosh HD:Users:daniel:Documents:Dokumente:EIT:Rennes:PEV:PEV_I:testResults:IncMlt.csv" decimal="," thousands="." tab="0" semicolon="1">
+    <textPr fileType="mac" firstRow="11" sourceFile="Macintosh HD:Users:daniel:Documents:Dokumente:EIT:Rennes:PEV:PEV_I:testResults:IncMlt.csv" decimal="," thousands="." tab="0" semicolon="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -57,7 +57,7 @@
     </textPr>
   </connection>
   <connection id="4" name="IncMrt.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="11" sourceFile="Macintosh HD:Users:daniel:Documents:Dokumente:EIT:Rennes:PEV:PEV_I:testResults:IncMrt.csv" decimal="," thousands="." tab="0" semicolon="1">
+    <textPr fileType="mac" firstRow="11" sourceFile="Macintosh HD:Users:daniel:Documents:Dokumente:EIT:Rennes:PEV:PEV_I:testResults:IncMrt.csv" decimal="," thousands="." tab="0" semicolon="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -419,46 +419,81 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2133554136"/>
-        <c:axId val="2137047464"/>
+        <c:axId val="2082593640"/>
+        <c:axId val="2082598552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2133554136"/>
+        <c:axId val="2082593640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="160.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Delta</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137047464"/>
+        <c:crossAx val="2082598552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2137047464"/>
+        <c:axId val="2082598552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="2.0E-6"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Unavailability</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133554136"/>
+        <c:crossAx val="2082593640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -722,46 +757,81 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2123620120"/>
-        <c:axId val="-2123521560"/>
+        <c:axId val="2082506040"/>
+        <c:axId val="2082503080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2123620120"/>
+        <c:axId val="2082506040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="160.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Delta</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123521560"/>
+        <c:crossAx val="2082503080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2123521560"/>
+        <c:axId val="2082503080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.0052"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Unavailability</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123620120"/>
+        <c:crossAx val="2082506040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1445,46 +1515,81 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2136459624"/>
-        <c:axId val="-2136757256"/>
+        <c:axId val="2084014216"/>
+        <c:axId val="2084017176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2136459624"/>
+        <c:axId val="2084014216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>MLT</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136757256"/>
+        <c:crossAx val="2084017176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2136757256"/>
+        <c:axId val="2084017176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="3.1E-6"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Unavailability</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136459624"/>
+        <c:crossAx val="2084014216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2168,46 +2273,79 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2113390344"/>
-        <c:axId val="-2113385464"/>
+        <c:axId val="2084046152"/>
+        <c:axId val="2084049112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2113390344"/>
+        <c:axId val="2084046152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>MLT</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113385464"/>
+        <c:crossAx val="2084049112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2113385464"/>
+        <c:axId val="2084049112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Unavailability</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113390344"/>
+        <c:crossAx val="2084046152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2891,46 +3029,81 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2113754760"/>
-        <c:axId val="-2113748808"/>
+        <c:axId val="2081618328"/>
+        <c:axId val="2081593528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2113754760"/>
+        <c:axId val="2081618328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="500.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>MRT</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113748808"/>
+        <c:crossAx val="2081593528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2113748808"/>
+        <c:axId val="2081593528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.0007"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Unavailability</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113754760"/>
+        <c:crossAx val="2081618328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3614,46 +3787,80 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2113228328"/>
-        <c:axId val="-2104947032"/>
+        <c:axId val="2081563384"/>
+        <c:axId val="2081560424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2113228328"/>
+        <c:axId val="2081563384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="500.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>MRT</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104947032"/>
+        <c:crossAx val="2081560424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2104947032"/>
+        <c:axId val="2081560424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Unavailability</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113228328"/>
+        <c:crossAx val="2081563384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3711,10 +3918,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>incD!$A$2:$A$22</c:f>
+              <c:f>incD!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>80.0</c:v>
                 </c:pt>
@@ -3774,19 +3981,16 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>99.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>100.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>incD!$B$2:$B$22</c:f>
+              <c:f>incD!$B$2:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>3E-6</c:v>
                 </c:pt>
@@ -3846,9 +4050,6 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>1.0E-6</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9E-6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3863,46 +4064,86 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2112640392"/>
-        <c:axId val="-2112467624"/>
+        <c:axId val="2081513960"/>
+        <c:axId val="2081511000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2112640392"/>
+        <c:axId val="2081513960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100.0"/>
+          <c:min val="65.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>d</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t>etection probability in percent</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112467624"/>
+        <c:crossAx val="2081511000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2112467624"/>
+        <c:axId val="2081511000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Unavailability</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112640392"/>
+        <c:crossAx val="2081513960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3960,10 +4201,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>incD!$A$2:$A$22</c:f>
+              <c:f>incD!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>80.0</c:v>
                 </c:pt>
@@ -4023,19 +4264,16 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>99.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>100.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>incD!$C$2:$C$22</c:f>
+              <c:f>incD!$C$2:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.005247</c:v>
                 </c:pt>
@@ -4095,9 +4333,6 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0.00503</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.005609</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4112,46 +4347,81 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2112117000"/>
-        <c:axId val="-2112391336"/>
+        <c:axId val="2081483048"/>
+        <c:axId val="2081480088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2112117000"/>
+        <c:axId val="2081483048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100.0"/>
+          <c:min val="65.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>detection probability in percent</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112391336"/>
+        <c:crossAx val="2081480088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2112391336"/>
+        <c:axId val="2081480088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Unavailability</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112117000"/>
+        <c:crossAx val="2081483048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4363,16 +4633,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4394,15 +4664,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4764,8 +5034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5132,8 +5402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6269,8 +6539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7404,10 +7674,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7647,17 +7917,6 @@
         <v>5.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22">
-        <v>100</v>
-      </c>
-      <c r="B22">
-        <v>9.0000000000000002E-6</v>
-      </c>
-      <c r="C22">
-        <v>5.6090000000000003E-3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>